<commit_message>
Implement scenario driven by spending inputs
</commit_message>
<xml_diff>
--- a/autumn/xls/spending_inputs_fiji.xlsx
+++ b/autumn/xls/spending_inputs_fiji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Models\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC88C38A-B698-41A3-80A6-0241D2714A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA77FB-BAF1-4733-8040-AF30A9C1E3BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10428" xr2:uid="{F77CEE3A-6CF7-424C-8718-5499A15CD008}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6108" xr2:uid="{F77CEE3A-6CF7-424C-8718-5499A15CD008}"/>
   </bookViews>
   <sheets>
     <sheet name="spending" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>spending_type</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>program</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative</t>
   </si>
 </sst>
 </file>
@@ -112,11 +115,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56380E46-6AD5-42C0-A050-89DCA9324B68}">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -456,92 +460,95 @@
         <v>3</v>
       </c>
       <c r="D1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E1" s="1">
         <v>2015</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2016</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2017</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2018</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2019</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2020</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>2021</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>2022</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>2023</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>2024</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>2025</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>2026</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>2027</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>2028</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="1">
         <v>2029</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>2030</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>2031</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="1">
         <v>2032</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>2033</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>2034</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>2035</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C2" s="4">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C3" s="4">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -553,20 +560,20 @@
         <v>2000000</v>
       </c>
       <c r="E4">
+        <v>2000000</v>
+      </c>
+      <c r="F4">
         <v>1000000</v>
       </c>
-      <c r="F4">
-        <v>500000</v>
-      </c>
       <c r="G4">
+        <v>500000</v>
+      </c>
+      <c r="H4">
         <v>2000000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1000000</v>
       </c>
-      <c r="I4">
-        <v>500000</v>
-      </c>
       <c r="J4">
         <v>500000</v>
       </c>
@@ -612,39 +619,50 @@
       <c r="X4">
         <v>500000</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C5" s="4">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C6" s="4">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
     </row>
   </sheetData>

</xml_diff>